<commit_message>
importing files and exporting files completed
</commit_message>
<xml_diff>
--- a/students_sample.xlsx
+++ b/students_sample.xlsx
@@ -10,13 +10,17 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="26">
   <si>
     <t>name</t>
   </si>
@@ -82,6 +86,18 @@
   </si>
   <si>
     <t>amali.14@cse.mrt.ac.lk</t>
+  </si>
+  <si>
+    <t>ashane2.14@cse.mrt.ac.lk</t>
+  </si>
+  <si>
+    <t>menuka2.14@cse.mrt.ac.lk</t>
+  </si>
+  <si>
+    <t>menuka7.14@cse.mrt.ac.lk</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -426,21 +442,217 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
   </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>7777777777</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>7777777777</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>7777777777</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>7777777777</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6">
+        <v>7777777777</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -473,7 +685,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C2">
         <v>7777777777</v>
@@ -491,130 +703,24 @@
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3">
-        <v>7777777777</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4">
-        <v>7777777777</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5">
-        <v>7777777777</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6">
-        <v>7777777777</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="A1:H1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
@@ -622,14 +728,224 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2">
+        <v>7777777777</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2">
+        <v>7777777777</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
email config and handled some possible inut s
</commit_message>
<xml_diff>
--- a/students_sample.xlsx
+++ b/students_sample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,13 +14,14 @@
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="15">
   <si>
     <t>name</t>
   </si>
@@ -49,9 +50,6 @@
     <t>Ashane</t>
   </si>
   <si>
-    <t>ashane.14@cse.mrt.ac.lk</t>
-  </si>
-  <si>
     <t>public</t>
   </si>
   <si>
@@ -64,40 +62,10 @@
     <t>Moratuwa</t>
   </si>
   <si>
-    <t>Menuka</t>
-  </si>
-  <si>
-    <t>Arunan</t>
-  </si>
-  <si>
-    <t>Prabodha</t>
-  </si>
-  <si>
-    <t>Amali</t>
-  </si>
-  <si>
-    <t>menuka.14@cse.mrt.ac.lk</t>
-  </si>
-  <si>
-    <t>arunan.14@cse.mrt.ac.lk</t>
-  </si>
-  <si>
-    <t>prabodha.14@cse.mrt.ac.lk</t>
-  </si>
-  <si>
-    <t>amali.14@cse.mrt.ac.lk</t>
-  </si>
-  <si>
-    <t>ashane2.14@cse.mrt.ac.lk</t>
-  </si>
-  <si>
-    <t>menuka2.14@cse.mrt.ac.lk</t>
-  </si>
-  <si>
-    <t>menuka7.14@cse.mrt.ac.lk</t>
-  </si>
-  <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>ashann.14@cse.mrt.ac.lk</t>
   </si>
 </sst>
 </file>
@@ -444,23 +412,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="23.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="36.85546875" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -495,150 +466,42 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D2">
         <v>7777777777</v>
       </c>
       <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>12</v>
       </c>
-      <c r="I2" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3">
-        <v>7777777777</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" t="s">
-        <v>13</v>
-      </c>
+      <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4">
-        <v>7777777777</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" t="s">
-        <v>13</v>
-      </c>
+      <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5">
-        <v>7777777777</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" t="s">
-        <v>13</v>
-      </c>
+      <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6">
-        <v>7777777777</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" t="s">
-        <v>13</v>
-      </c>
+      <c r="C6" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -649,10 +512,13 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -681,35 +547,9 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2">
-        <v>7777777777</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
+      <c r="B2" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -730,10 +570,105 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="C2" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="36.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="B2" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -769,15 +704,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -805,147 +743,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2">
-        <v>7777777777</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2">
-        <v>7777777777</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-  </hyperlinks>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>